<commit_message>
Some variables and functions are changed to a more understandable name and some unused lines are removed. Some other unused lines are commented.
</commit_message>
<xml_diff>
--- a/exlist.xlsx
+++ b/exlist.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sayfa3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -418,7 +418,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -433,10 +433,10 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>1300</v>
+        <v>1600</v>
       </c>
       <c r="C1" t="n">
-        <v>1311.517920006308</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="2">
@@ -446,10 +446,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="C2" t="n">
-        <v>1188.482079993692</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="3">
@@ -459,7 +459,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="4">
@@ -469,7 +469,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="5">
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="6">
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="7">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="9">
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="10">
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="11">
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="12">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="13">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="14">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="15">
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="16">
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="17">
@@ -599,7 +599,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="18">
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1200</v>
+        <v>1600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>